<commit_message>
Fixed load_data module not found problem
</commit_message>
<xml_diff>
--- a/tests/test_data/test_data.xlsx
+++ b/tests/test_data/test_data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Home Economics\Automobile Matters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samueldy\Box Sync\Coursework\MECHENG 599-006\Projects\course-project\pov_mileage_stats\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2052A965-54FF-4D90-AE72-945633775EC8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12750" xr2:uid="{4EAEBC70-2876-42F4-A6D5-02178DF92E82}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12750"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,13 +34,13 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Trip A</t>
+    <t>Miles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,61 +76,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -468,10 +413,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B800633C-4054-4545-85F9-0C41D439753B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1096"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -8498,7 +8445,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A1096">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A2=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>